<commit_message>
Revise analysis of chlorides and add simplified analysis notebook
</commit_message>
<xml_diff>
--- a/Derived_Data/Site_IC_Data.xlsx
+++ b/Derived_Data/Site_IC_Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\curtis.bohlen\Dropbox\Work\LCWMD Data\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\curtis.bohlen\Documents\State of the Bay 2020\Data\A3. Stormwater\LCWMD_Monitoring\Derived_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="4810"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19185" windowHeight="4815"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -483,18 +483,18 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.90625" customWidth="1"/>
-    <col min="3" max="7" width="16.08984375" customWidth="1"/>
-    <col min="8" max="8" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -520,7 +520,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -546,11 +546,11 @@
         <v>0.20202718267680259</v>
       </c>
       <c r="H2" s="5">
-        <f>F2/E2</f>
+        <f t="shared" ref="H2:H8" si="0">F2/E2</f>
         <v>0.20202718267680259</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -572,15 +572,15 @@
         <v>80.2</v>
       </c>
       <c r="G3" s="5">
-        <f t="shared" ref="G3:G8" si="0">D3/C3</f>
+        <f t="shared" ref="G3:G8" si="1">D3/C3</f>
         <v>0.12866998235199745</v>
       </c>
       <c r="H3" s="5">
-        <f>F3/E3</f>
+        <f t="shared" si="0"/>
         <v>0.12866998235199745</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -594,23 +594,23 @@
         <v>53.6</v>
       </c>
       <c r="E4" s="4">
-        <f>E3+C4</f>
-        <v>901.9</v>
+        <f>E3+C4 +C2</f>
+        <v>1336</v>
       </c>
       <c r="F4" s="4">
-        <f>F3+D4</f>
-        <v>133.80000000000001</v>
+        <f>F3+D4+D2</f>
+        <v>221.5</v>
       </c>
       <c r="G4" s="5">
+        <f t="shared" si="1"/>
+        <v>0.19239052404881549</v>
+      </c>
+      <c r="H4" s="5">
         <f t="shared" si="0"/>
-        <v>0.19239052404881549</v>
-      </c>
-      <c r="H4" s="5">
-        <f>F4/E4</f>
-        <v>0.14835347599512141</v>
+        <v>0.1657934131736527</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -625,22 +625,22 @@
       </c>
       <c r="E5" s="4">
         <f>E4+C5</f>
-        <v>1006.9</v>
+        <v>1441</v>
       </c>
       <c r="F5" s="4">
         <f>F4+D5</f>
-        <v>198.9</v>
+        <v>286.60000000000002</v>
       </c>
       <c r="G5" s="5">
+        <f t="shared" si="1"/>
+        <v>0.62</v>
+      </c>
+      <c r="H5" s="5">
         <f t="shared" si="0"/>
-        <v>0.62</v>
-      </c>
-      <c r="H5" s="5">
-        <f>F5/E5</f>
-        <v>0.19753699473631942</v>
+        <v>0.19888965995836227</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -654,23 +654,23 @@
         <v>123</v>
       </c>
       <c r="E6" s="4">
-        <f>C6</f>
+        <f t="shared" ref="E6:F8" si="2">C6</f>
         <v>298.5</v>
       </c>
       <c r="F6" s="4">
-        <f>D6</f>
+        <f t="shared" si="2"/>
         <v>123</v>
       </c>
       <c r="G6" s="5">
+        <f t="shared" si="1"/>
+        <v>0.4120603015075377</v>
+      </c>
+      <c r="H6" s="5">
         <f t="shared" si="0"/>
         <v>0.4120603015075377</v>
       </c>
-      <c r="H6" s="5">
-        <f>F6/E6</f>
-        <v>0.4120603015075377</v>
-      </c>
     </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -684,23 +684,23 @@
         <v>44.7</v>
       </c>
       <c r="E7" s="4">
-        <f>C7</f>
+        <f t="shared" si="2"/>
         <v>137.30000000000001</v>
       </c>
       <c r="F7" s="4">
-        <f>D7</f>
+        <f t="shared" si="2"/>
         <v>44.7</v>
       </c>
       <c r="G7" s="5">
+        <f t="shared" si="1"/>
+        <v>0.32556445739257101</v>
+      </c>
+      <c r="H7" s="5">
         <f t="shared" si="0"/>
         <v>0.32556445739257101</v>
       </c>
-      <c r="H7" s="5">
-        <f>F7/E7</f>
-        <v>0.32556445739257101</v>
-      </c>
     </row>
-    <row r="8" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
@@ -714,19 +714,19 @@
         <v>239.7</v>
       </c>
       <c r="E8" s="4">
-        <f>C8</f>
+        <f t="shared" si="2"/>
         <v>427.4</v>
       </c>
       <c r="F8" s="4">
-        <f>D8</f>
+        <f t="shared" si="2"/>
         <v>239.7</v>
       </c>
       <c r="G8" s="5">
+        <f t="shared" si="1"/>
+        <v>0.56083294337856804</v>
+      </c>
+      <c r="H8" s="5">
         <f t="shared" si="0"/>
-        <v>0.56083294337856804</v>
-      </c>
-      <c r="H8" s="5">
-        <f>F8/E8</f>
         <v>0.56083294337856804</v>
       </c>
     </row>

</xml_diff>